<commit_message>
Updates to facilitate normalization updates on database records.
</commit_message>
<xml_diff>
--- a/input/qa_template_map.xlsx
+++ b/input/qa_template_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B38AA458-4E3A-4181-ADD2-465BC91EE098}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4FE5966-2628-41B0-AB9F-B77F2B7CBBE5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
+    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="11235" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="114">
   <si>
     <t>from</t>
   </si>
@@ -261,9 +261,6 @@
     <t>dose_level_original</t>
   </si>
   <si>
-    <t>dose_level_original_units</t>
-  </si>
-  <si>
     <t>administration_route_original</t>
   </si>
   <si>
@@ -361,6 +358,27 @@
   </si>
   <si>
     <t>conc_bound_type</t>
+  </si>
+  <si>
+    <t>dose_level_units_original</t>
+  </si>
+  <si>
+    <t>flow_rate</t>
+  </si>
+  <si>
+    <t>flow_rate_units</t>
+  </si>
+  <si>
+    <t>chamber_size</t>
+  </si>
+  <si>
+    <t>chamber_size_units</t>
+  </si>
+  <si>
+    <t>test_environment_temperature</t>
+  </si>
+  <si>
+    <t>test_environment_humidity</t>
   </si>
 </sst>
 </file>
@@ -721,20 +739,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -745,64 +763,64 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -811,9 +829,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
         <v>66</v>
@@ -822,9 +840,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -833,64 +851,64 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="s">
         <v>100</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
@@ -899,20 +917,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -921,20 +939,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -943,9 +961,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -954,9 +972,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -965,9 +983,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
@@ -976,53 +994,53 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
         <v>100</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>85</v>
-      </c>
-      <c r="B25" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -1031,9 +1049,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -1042,9 +1060,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -1053,42 +1071,42 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B33" t="s">
         <v>60</v>
@@ -1097,9 +1115,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B34" t="s">
         <v>23</v>
@@ -1108,42 +1126,42 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
@@ -1152,9 +1170,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B39" t="s">
         <v>46</v>
@@ -1163,9 +1181,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" t="s">
         <v>48</v>
@@ -1174,9 +1192,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
         <v>47</v>
@@ -1185,9 +1203,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B42" t="s">
         <v>62</v>
@@ -1196,9 +1214,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
         <v>63</v>
@@ -1207,9 +1225,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
@@ -1218,9 +1236,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B45" t="s">
         <v>58</v>
@@ -1229,9 +1247,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B46" t="s">
         <v>59</v>
@@ -1240,9 +1258,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
         <v>55</v>
@@ -1251,20 +1269,20 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C48" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
         <v>56</v>
@@ -1273,9 +1291,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
         <v>57</v>
@@ -1284,9 +1302,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B51" t="s">
         <v>64</v>
@@ -1295,42 +1313,42 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C52" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B53" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" t="s">
         <v>100</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" t="s">
-        <v>101</v>
-      </c>
-      <c r="C54" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B55" t="s">
         <v>61</v>
@@ -1339,20 +1357,20 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C56" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B57" t="s">
         <v>50</v>
@@ -1361,9 +1379,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B58" t="s">
         <v>49</v>
@@ -1372,9 +1390,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B59" t="s">
         <v>52</v>
@@ -1383,9 +1401,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
         <v>51</v>
@@ -1394,42 +1412,42 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C61" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C62" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B63" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C63" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B64" t="s">
         <v>31</v>
@@ -1438,9 +1456,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B65" t="s">
         <v>32</v>
@@ -1449,9 +1467,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B66" t="s">
         <v>29</v>
@@ -1460,9 +1478,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B67" t="s">
         <v>28</v>
@@ -1471,9 +1489,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B68" t="s">
         <v>30</v>
@@ -1482,9 +1500,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B69" t="s">
         <v>23</v>
@@ -1493,9 +1511,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B70" t="s">
         <v>9</v>
@@ -1504,9 +1522,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B71" t="s">
         <v>26</v>
@@ -1515,9 +1533,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B72" t="s">
         <v>27</v>
@@ -1526,9 +1544,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B73" t="s">
         <v>24</v>
@@ -1537,9 +1555,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B74" t="s">
         <v>25</v>
@@ -1548,9 +1566,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B75" t="s">
         <v>18</v>
@@ -1559,9 +1577,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B76" t="s">
         <v>19</v>
@@ -1570,9 +1588,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B77" t="s">
         <v>73</v>
@@ -1581,20 +1599,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B78" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="C78" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B79" t="s">
         <v>20</v>
@@ -1603,9 +1621,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B80" t="s">
         <v>21</v>
@@ -1614,20 +1632,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B81" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C81" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B82" t="s">
         <v>22</v>
@@ -1636,20 +1654,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C83" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B84" t="s">
         <v>11</v>
@@ -1658,53 +1676,53 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C85" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B86" t="s">
+        <v>99</v>
+      </c>
+      <c r="C86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
         <v>100</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>86</v>
-      </c>
-      <c r="B87" t="s">
-        <v>101</v>
-      </c>
-      <c r="C87" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C88" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B89" t="s">
         <v>72</v>
@@ -1713,20 +1731,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B90" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C90" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B91" t="s">
         <v>36</v>
@@ -1735,9 +1753,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B92" t="s">
         <v>38</v>
@@ -1746,9 +1764,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B93" t="s">
         <v>37</v>
@@ -1757,9 +1775,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B94" t="s">
         <v>9</v>
@@ -1768,9 +1786,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B95" t="s">
         <v>39</v>
@@ -1779,9 +1797,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B96" t="s">
         <v>40</v>
@@ -1790,9 +1808,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B97" t="s">
         <v>11</v>
@@ -1801,42 +1819,42 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B98" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C98" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B99" t="s">
+        <v>99</v>
+      </c>
+      <c r="C99" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>86</v>
+      </c>
+      <c r="B100" t="s">
         <v>100</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>87</v>
-      </c>
-      <c r="B100" t="s">
-        <v>101</v>
-      </c>
-      <c r="C100" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B101" t="s">
         <v>35</v>
@@ -1845,9 +1863,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B102" t="s">
         <v>33</v>
@@ -1856,9 +1874,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B103" t="s">
         <v>34</v>
@@ -1867,9 +1885,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B104" t="s">
         <v>41</v>
@@ -1878,15 +1896,81 @@
         <v>41</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B105" t="s">
         <v>42</v>
       </c>
       <c r="C105" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>85</v>
+      </c>
+      <c r="B106" t="s">
+        <v>108</v>
+      </c>
+      <c r="C106" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>85</v>
+      </c>
+      <c r="B107" t="s">
+        <v>109</v>
+      </c>
+      <c r="C107" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>85</v>
+      </c>
+      <c r="B108" t="s">
+        <v>110</v>
+      </c>
+      <c r="C108" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>85</v>
+      </c>
+      <c r="B109" t="s">
+        <v>111</v>
+      </c>
+      <c r="C109" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>85</v>
+      </c>
+      <c r="B110" t="s">
+        <v>112</v>
+      </c>
+      <c r="C110" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>85</v>
+      </c>
+      <c r="B111" t="s">
+        <v>113</v>
+      </c>
+      <c r="C111" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update field pH to ph
</commit_message>
<xml_diff>
--- a/input/qa_template_map.xlsx
+++ b/input/qa_template_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4FE5966-2628-41B0-AB9F-B77F2B7CBBE5}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F99F787B-76AA-4FF0-8D86-5A612583EF04}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="11235" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,9 +114,6 @@
     <t>dermal_dose_vehicle</t>
   </si>
   <si>
-    <t>dermal_dose_vehicle_pH</t>
-  </si>
-  <si>
     <t>dermal_applied_area</t>
   </si>
   <si>
@@ -379,6 +376,9 @@
   </si>
   <si>
     <t>test_environment_humidity</t>
+  </si>
+  <si>
+    <t>dermal_dose_vehicle_ph</t>
   </si>
 </sst>
 </file>
@@ -741,18 +741,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
   <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -763,64 +763,64 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
         <v>81</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -829,20 +829,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -851,64 +851,64 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
@@ -917,20 +917,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -939,20 +939,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -961,9 +961,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -972,9 +972,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -983,9 +983,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
@@ -994,53 +994,53 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" t="s">
         <v>99</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>84</v>
-      </c>
-      <c r="B26" t="s">
-        <v>100</v>
-      </c>
-      <c r="C26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -1049,9 +1049,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -1060,9 +1060,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -1071,53 +1071,53 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" t="s">
         <v>102</v>
       </c>
-      <c r="C30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>87</v>
-      </c>
-      <c r="B32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B34" t="s">
         <v>23</v>
@@ -1126,42 +1126,42 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
@@ -1170,64 +1170,64 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" t="s">
         <v>46</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>87</v>
-      </c>
-      <c r="B40" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>87</v>
-      </c>
-      <c r="B41" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
         <v>62</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
@@ -1236,273 +1236,273 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" t="s">
         <v>58</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" t="s">
         <v>55</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C49" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>87</v>
-      </c>
-      <c r="B48" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" t="s">
         <v>56</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>87</v>
-      </c>
-      <c r="B50" t="s">
-        <v>57</v>
-      </c>
-      <c r="C50" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B53" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" t="s">
         <v>99</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>87</v>
-      </c>
-      <c r="B54" t="s">
-        <v>100</v>
-      </c>
-      <c r="C54" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C55" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C56" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B57" t="s">
+        <v>49</v>
+      </c>
+      <c r="C57" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>86</v>
+      </c>
+      <c r="B59" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>86</v>
+      </c>
+      <c r="B60" t="s">
         <v>50</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C60" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>87</v>
-      </c>
-      <c r="B58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C58" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>87</v>
-      </c>
-      <c r="B59" t="s">
-        <v>52</v>
-      </c>
-      <c r="C59" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>87</v>
-      </c>
-      <c r="B60" t="s">
-        <v>51</v>
-      </c>
-      <c r="C60" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C61" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C62" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C63" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B64" t="s">
+        <v>30</v>
+      </c>
+      <c r="C64" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" t="s">
         <v>31</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>85</v>
-      </c>
-      <c r="B65" t="s">
-        <v>32</v>
-      </c>
-      <c r="C65" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B66" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" t="s">
         <v>29</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C68" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>85</v>
-      </c>
-      <c r="B67" t="s">
-        <v>28</v>
-      </c>
-      <c r="C67" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>85</v>
-      </c>
-      <c r="B68" t="s">
-        <v>30</v>
-      </c>
-      <c r="C68" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B69" t="s">
         <v>23</v>
@@ -1511,9 +1511,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B70" t="s">
         <v>9</v>
@@ -1522,31 +1522,31 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B71" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>84</v>
+      </c>
+      <c r="B72" t="s">
         <v>26</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>85</v>
-      </c>
-      <c r="B72" t="s">
-        <v>27</v>
-      </c>
-      <c r="C72" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B73" t="s">
         <v>24</v>
@@ -1555,20 +1555,20 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B74" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="C74" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B75" t="s">
         <v>18</v>
@@ -1577,9 +1577,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B76" t="s">
         <v>19</v>
@@ -1588,31 +1588,31 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B77" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C77" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B78" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C78" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B79" t="s">
         <v>20</v>
@@ -1621,9 +1621,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B80" t="s">
         <v>21</v>
@@ -1632,20 +1632,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B81" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C81" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B82" t="s">
         <v>22</v>
@@ -1654,20 +1654,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C83" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B84" t="s">
         <v>11</v>
@@ -1676,108 +1676,108 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C85" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86" t="s">
+        <v>98</v>
+      </c>
+      <c r="C86" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>84</v>
+      </c>
+      <c r="B87" t="s">
         <v>99</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>85</v>
-      </c>
-      <c r="B87" t="s">
-        <v>100</v>
-      </c>
-      <c r="C87" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B88" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C88" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B89" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C89" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B90" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C90" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B91" t="s">
+        <v>35</v>
+      </c>
+      <c r="C91" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>85</v>
+      </c>
+      <c r="B92" t="s">
+        <v>37</v>
+      </c>
+      <c r="C92" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>85</v>
+      </c>
+      <c r="B93" t="s">
         <v>36</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C93" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>86</v>
-      </c>
-      <c r="B92" t="s">
-        <v>38</v>
-      </c>
-      <c r="C92" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>86</v>
-      </c>
-      <c r="B93" t="s">
-        <v>37</v>
-      </c>
-      <c r="C93" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B94" t="s">
         <v>9</v>
@@ -1786,31 +1786,31 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B95" t="s">
+        <v>38</v>
+      </c>
+      <c r="C95" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>85</v>
+      </c>
+      <c r="B96" t="s">
         <v>39</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>86</v>
-      </c>
-      <c r="B96" t="s">
-        <v>40</v>
-      </c>
-      <c r="C96" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B97" t="s">
         <v>11</v>
@@ -1819,158 +1819,158 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B98" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C98" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B99" t="s">
+        <v>98</v>
+      </c>
+      <c r="C99" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>85</v>
+      </c>
+      <c r="B100" t="s">
         <v>99</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>86</v>
-      </c>
-      <c r="B100" t="s">
-        <v>100</v>
-      </c>
-      <c r="C100" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B101" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C101" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B102" t="s">
+        <v>32</v>
+      </c>
+      <c r="C102" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>85</v>
+      </c>
+      <c r="B103" t="s">
         <v>33</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C103" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>86</v>
-      </c>
-      <c r="B103" t="s">
-        <v>34</v>
-      </c>
-      <c r="C103" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B104" t="s">
+        <v>40</v>
+      </c>
+      <c r="C104" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>85</v>
+      </c>
+      <c r="B105" t="s">
         <v>41</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C105" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>86</v>
-      </c>
-      <c r="B105" t="s">
-        <v>42</v>
-      </c>
-      <c r="C105" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B106" t="s">
+        <v>107</v>
+      </c>
+      <c r="C106" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>84</v>
+      </c>
+      <c r="B107" t="s">
         <v>108</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C107" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>85</v>
-      </c>
-      <c r="B107" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>84</v>
+      </c>
+      <c r="B108" t="s">
         <v>109</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C108" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>85</v>
-      </c>
-      <c r="B108" t="s">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>84</v>
+      </c>
+      <c r="B109" t="s">
         <v>110</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C109" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>85</v>
-      </c>
-      <c r="B109" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>84</v>
+      </c>
+      <c r="B110" t="s">
         <v>111</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C110" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>85</v>
-      </c>
-      <c r="B110" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>84</v>
+      </c>
+      <c r="B111" t="s">
         <v>112</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C111" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>85</v>
-      </c>
-      <c r="B111" t="s">
-        <v>113</v>
-      </c>
-      <c r="C111" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to QC template and map.
</commit_message>
<xml_diff>
--- a/input/qa_template_map.xlsx
+++ b/input/qa_template_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F99F787B-76AA-4FF0-8D86-5A612583EF04}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29D3768F-7131-43C9-B987-A5E72F634437}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$105</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="119">
   <si>
     <t>from</t>
   </si>
@@ -379,6 +379,21 @@
   </si>
   <si>
     <t>dermal_dose_vehicle_ph</t>
+  </si>
+  <si>
+    <t>administration_form_original</t>
+  </si>
+  <si>
+    <t>administration_form</t>
+  </si>
+  <si>
+    <t>administration_method_original</t>
+  </si>
+  <si>
+    <t>administration_method</t>
+  </si>
+  <si>
+    <t>dose_frequency_original</t>
   </si>
 </sst>
 </file>
@@ -739,20 +754,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -763,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -774,7 +789,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -785,7 +800,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -796,7 +811,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -807,7 +822,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -818,7 +833,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -829,7 +844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -840,7 +855,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -851,7 +866,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -862,7 +877,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -873,7 +888,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -884,7 +899,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -895,7 +910,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -906,7 +921,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -917,7 +932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -928,7 +943,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -939,7 +954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -950,7 +965,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -961,7 +976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -972,7 +987,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -983,7 +998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>83</v>
       </c>
@@ -994,7 +1009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>83</v>
       </c>
@@ -1005,7 +1020,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>83</v>
       </c>
@@ -1016,7 +1031,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -1027,7 +1042,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -1038,7 +1053,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -1049,7 +1064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -1060,7 +1075,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -1071,7 +1086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -1082,7 +1097,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -1093,7 +1108,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -1104,7 +1119,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -1115,7 +1130,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -1126,7 +1141,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -1137,7 +1152,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -1148,7 +1163,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -1159,7 +1174,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>86</v>
       </c>
@@ -1170,7 +1185,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -1181,7 +1196,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -1192,7 +1207,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -1203,7 +1218,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -1214,7 +1229,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -1225,7 +1240,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -1236,7 +1251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -1247,7 +1262,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -1258,7 +1273,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -1269,7 +1284,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -1280,7 +1295,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -1291,7 +1306,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -1302,7 +1317,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -1313,7 +1328,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -1324,7 +1339,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>86</v>
       </c>
@@ -1335,7 +1350,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -1346,7 +1361,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>86</v>
       </c>
@@ -1357,7 +1372,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -1368,7 +1383,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>86</v>
       </c>
@@ -1379,7 +1394,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>86</v>
       </c>
@@ -1390,7 +1405,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>86</v>
       </c>
@@ -1401,7 +1416,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -1412,7 +1427,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>84</v>
       </c>
@@ -1423,7 +1438,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>84</v>
       </c>
@@ -1434,7 +1449,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>84</v>
       </c>
@@ -1445,7 +1460,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>84</v>
       </c>
@@ -1456,7 +1471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>84</v>
       </c>
@@ -1467,7 +1482,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>84</v>
       </c>
@@ -1478,7 +1493,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>84</v>
       </c>
@@ -1489,7 +1504,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>84</v>
       </c>
@@ -1500,7 +1515,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -1511,7 +1526,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>84</v>
       </c>
@@ -1522,7 +1537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>84</v>
       </c>
@@ -1533,7 +1548,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>84</v>
       </c>
@@ -1544,7 +1559,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>84</v>
       </c>
@@ -1555,7 +1570,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>84</v>
       </c>
@@ -1566,7 +1581,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -1577,412 +1592,434 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>84</v>
       </c>
       <c r="B76" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C76" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>84</v>
       </c>
       <c r="B77" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C77" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>84</v>
       </c>
       <c r="B78" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="C78" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>84</v>
       </c>
       <c r="B79" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C79" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>84</v>
       </c>
       <c r="B80" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="C80" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>84</v>
       </c>
       <c r="B81" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="C81" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="C82" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="C83" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="C84" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C85" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C86" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>84</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C87" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>84</v>
       </c>
       <c r="B88" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C88" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>84</v>
       </c>
       <c r="B89" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="C89" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B90" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C90" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>85</v>
       </c>
       <c r="B91" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C91" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>85</v>
       </c>
       <c r="B92" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C92" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>85</v>
       </c>
       <c r="B93" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="C93" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>85</v>
       </c>
       <c r="B94" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C94" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>85</v>
       </c>
       <c r="B95" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C95" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>85</v>
       </c>
       <c r="B96" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="C96" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>85</v>
       </c>
       <c r="B97" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="C97" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>85</v>
       </c>
       <c r="B98" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C98" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>85</v>
       </c>
       <c r="B99" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C99" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>85</v>
       </c>
       <c r="B100" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="C100" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>85</v>
       </c>
       <c r="B101" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C101" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>85</v>
       </c>
       <c r="B102" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C102" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>85</v>
       </c>
       <c r="B103" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C103" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>85</v>
       </c>
       <c r="B104" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C104" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B105" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="C105" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>84</v>
       </c>
       <c r="B106" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C106" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>84</v>
       </c>
       <c r="B107" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C107" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>84</v>
       </c>
       <c r="B108" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C108" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>84</v>
       </c>
       <c r="B109" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C109" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>84</v>
       </c>
       <c r="B110" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C110" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>84</v>
       </c>
       <c r="B111" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C111" t="s">
-        <v>112</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>84</v>
+      </c>
+      <c r="B112" t="s">
+        <v>116</v>
+      </c>
+      <c r="C112" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>84</v>
+      </c>
+      <c r="B113" t="s">
+        <v>118</v>
+      </c>
+      <c r="C113" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C105" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C105">
-      <sortCondition ref="A2:A105"/>
-      <sortCondition ref="B2:B105"/>
+  <autoFilter ref="A1:C104" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C104">
+      <sortCondition ref="A2:A104"/>
+      <sortCondition ref="B2:B104"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C105">
-    <sortCondition ref="A2:A105"/>
-    <sortCondition ref="B2:B105"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C104">
+    <sortCondition ref="A2:A104"/>
+    <sortCondition ref="B2:B104"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated qa_template values, added qc_validation rules, added field mapping
</commit_message>
<xml_diff>
--- a/input/qa_template_map.xlsx
+++ b/input/qa_template_map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/kesic_branislav_epa_gov/Documents/Profile/Documents/GitHub/CvTdbLoad/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29D3768F-7131-43C9-B987-A5E72F634437}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF0240BC-529C-425C-938B-2D50F4D29F08}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="119">
   <si>
     <t>from</t>
   </si>
@@ -754,20 +754,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:C118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -778,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -789,7 +789,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -800,7 +800,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -811,7 +811,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -822,7 +822,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -833,7 +833,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -844,7 +844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -855,7 +855,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -866,7 +866,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -877,7 +877,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -888,7 +888,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -899,7 +899,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -910,7 +910,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -921,7 +921,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -932,7 +932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -943,7 +943,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -954,7 +954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -965,7 +965,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -976,7 +976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -987,7 +987,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -998,7 +998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>83</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>83</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>83</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>86</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>86</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>86</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>86</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>86</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>86</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>84</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>84</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>84</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>84</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>84</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>84</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>84</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>84</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>84</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>84</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>84</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>84</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>84</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>84</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>84</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>84</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>84</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>84</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>84</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>84</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>84</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>85</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>85</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>85</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>85</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>85</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>85</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>85</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>85</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>85</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>85</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>85</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>85</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>85</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>85</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>85</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>84</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>84</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>84</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>84</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>84</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>84</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>84</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>84</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>84</v>
       </c>
@@ -2008,6 +2008,61 @@
       </c>
       <c r="C113" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>84</v>
+      </c>
+      <c r="B114" t="s">
+        <v>27</v>
+      </c>
+      <c r="C114" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>84</v>
+      </c>
+      <c r="B115" t="s">
+        <v>28</v>
+      </c>
+      <c r="C115" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>84</v>
+      </c>
+      <c r="B116" t="s">
+        <v>29</v>
+      </c>
+      <c r="C116" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>84</v>
+      </c>
+      <c r="B117" t="s">
+        <v>30</v>
+      </c>
+      <c r="C117" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>84</v>
+      </c>
+      <c r="B118" t="s">
+        <v>31</v>
+      </c>
+      <c r="C118" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed qa_template duplicate, failproofed QC rules, fixed download_jira error, added bulk validation, improved qc_to_db
</commit_message>
<xml_diff>
--- a/input/qa_template_map.xlsx
+++ b/input/qa_template_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/kesic_branislav_epa_gov/Documents/Profile/Documents/GitHub/CvTdbLoad/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF0240BC-529C-425C-938B-2D50F4D29F08}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F09ACD3-E90A-4639-A017-BA03A96017E8}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="119">
   <si>
     <t>from</t>
   </si>
@@ -754,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C118"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C118" sqref="A114:C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2008,61 +2008,6 @@
       </c>
       <c r="C113" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
-        <v>84</v>
-      </c>
-      <c r="B114" t="s">
-        <v>27</v>
-      </c>
-      <c r="C114" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
-        <v>84</v>
-      </c>
-      <c r="B115" t="s">
-        <v>28</v>
-      </c>
-      <c r="C115" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
-        <v>84</v>
-      </c>
-      <c r="B116" t="s">
-        <v>29</v>
-      </c>
-      <c r="C116" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
-        <v>84</v>
-      </c>
-      <c r="B117" t="s">
-        <v>30</v>
-      </c>
-      <c r="C117" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
-        <v>84</v>
-      </c>
-      <c r="B118" t="s">
-        <v>31</v>
-      </c>
-      <c r="C118" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed duplicate fields in blank templates, Minor bug fixes, Logging improvements
</commit_message>
<xml_diff>
--- a/input/qa_template_map.xlsx
+++ b/input/qa_template_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/kesic_branislav_epa_gov/Documents/Profile/Documents/GitHub/CvTdbLoad/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F09ACD3-E90A-4639-A017-BA03A96017E8}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6982ED5-C4D0-40C8-8CCB-092C0D8DCD3B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$107</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="122">
   <si>
     <t>from</t>
   </si>
@@ -394,6 +394,15 @@
   </si>
   <si>
     <t>dose_frequency_original</t>
+  </si>
+  <si>
+    <t>effects_data</t>
+  </si>
+  <si>
+    <t>tk_params</t>
+  </si>
+  <si>
+    <t>httk_data</t>
   </si>
 </sst>
 </file>
@@ -754,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C118" sqref="A114:C118"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1088,35 +1097,35 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1124,10 +1133,10 @@
         <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -1135,10 +1144,10 @@
         <v>86</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -1146,10 +1155,10 @@
         <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1157,10 +1166,10 @@
         <v>86</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1168,10 +1177,10 @@
         <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1179,10 +1188,10 @@
         <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1190,10 +1199,10 @@
         <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -1201,10 +1210,10 @@
         <v>86</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -1212,10 +1221,10 @@
         <v>86</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -1223,10 +1232,10 @@
         <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -1234,10 +1243,10 @@
         <v>86</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -1245,10 +1254,10 @@
         <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -1256,10 +1265,10 @@
         <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -1267,10 +1276,10 @@
         <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -1278,10 +1287,10 @@
         <v>86</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -1289,10 +1298,10 @@
         <v>86</v>
       </c>
       <c r="B48" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1300,10 +1309,10 @@
         <v>86</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1311,10 +1320,10 @@
         <v>86</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -1322,10 +1331,10 @@
         <v>86</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="C51" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -1333,10 +1342,10 @@
         <v>86</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -1344,10 +1353,10 @@
         <v>86</v>
       </c>
       <c r="B53" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1355,10 +1364,10 @@
         <v>86</v>
       </c>
       <c r="B54" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="C54" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1366,10 +1375,10 @@
         <v>86</v>
       </c>
       <c r="B55" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C55" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -1377,10 +1386,10 @@
         <v>86</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C56" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -1388,10 +1397,10 @@
         <v>86</v>
       </c>
       <c r="B57" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="C57" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -1399,10 +1408,10 @@
         <v>86</v>
       </c>
       <c r="B58" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C58" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -1410,10 +1419,10 @@
         <v>86</v>
       </c>
       <c r="B59" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="C59" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -1421,43 +1430,43 @@
         <v>86</v>
       </c>
       <c r="B60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B61" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="C61" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B62" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="C62" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="C63" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -1465,10 +1474,10 @@
         <v>84</v>
       </c>
       <c r="B64" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="C64" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -1476,10 +1485,10 @@
         <v>84</v>
       </c>
       <c r="B65" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="C65" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -1487,10 +1496,10 @@
         <v>84</v>
       </c>
       <c r="B66" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="C66" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -1498,10 +1507,10 @@
         <v>84</v>
       </c>
       <c r="B67" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C67" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -1509,10 +1518,10 @@
         <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C68" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -1520,10 +1529,10 @@
         <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -1531,10 +1540,10 @@
         <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C70" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -1542,10 +1551,10 @@
         <v>84</v>
       </c>
       <c r="B71" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C71" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -1553,10 +1562,10 @@
         <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C72" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -1564,10 +1573,10 @@
         <v>84</v>
       </c>
       <c r="B73" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C73" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -1575,10 +1584,10 @@
         <v>84</v>
       </c>
       <c r="B74" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="C74" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -1586,10 +1595,10 @@
         <v>84</v>
       </c>
       <c r="B75" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C75" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -1597,10 +1606,10 @@
         <v>84</v>
       </c>
       <c r="B76" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="C76" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -1608,10 +1617,10 @@
         <v>84</v>
       </c>
       <c r="B77" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C77" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -1619,10 +1628,10 @@
         <v>84</v>
       </c>
       <c r="B78" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C78" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -1630,10 +1639,10 @@
         <v>84</v>
       </c>
       <c r="B79" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="C79" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -1641,10 +1650,10 @@
         <v>84</v>
       </c>
       <c r="B80" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="C80" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -1652,10 +1661,10 @@
         <v>84</v>
       </c>
       <c r="B81" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C81" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -1663,10 +1672,10 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="C82" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -1674,10 +1683,10 @@
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="C83" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -1685,10 +1694,10 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="C84" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -1696,10 +1705,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C85" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -1707,10 +1716,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="C86" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -1718,10 +1727,10 @@
         <v>84</v>
       </c>
       <c r="B87" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C87" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -1729,10 +1738,10 @@
         <v>84</v>
       </c>
       <c r="B88" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="C88" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -1740,43 +1749,43 @@
         <v>84</v>
       </c>
       <c r="B89" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C89" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B90" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="C90" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B91" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="C91" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B92" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="C92" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -1784,10 +1793,10 @@
         <v>85</v>
       </c>
       <c r="B93" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C93" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -1795,10 +1804,10 @@
         <v>85</v>
       </c>
       <c r="B94" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C94" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -1806,10 +1815,10 @@
         <v>85</v>
       </c>
       <c r="B95" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C95" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -1817,10 +1826,10 @@
         <v>85</v>
       </c>
       <c r="B96" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C96" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -1828,10 +1837,10 @@
         <v>85</v>
       </c>
       <c r="B97" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="C97" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -1839,10 +1848,10 @@
         <v>85</v>
       </c>
       <c r="B98" t="s">
-        <v>98</v>
+        <v>39</v>
       </c>
       <c r="C98" t="s">
-        <v>98</v>
+        <v>39</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -1850,10 +1859,10 @@
         <v>85</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="C99" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -1861,10 +1870,10 @@
         <v>85</v>
       </c>
       <c r="B100" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="C100" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -1872,10 +1881,10 @@
         <v>85</v>
       </c>
       <c r="B101" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="C101" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -1883,10 +1892,10 @@
         <v>85</v>
       </c>
       <c r="B102" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="C102" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -1894,10 +1903,10 @@
         <v>85</v>
       </c>
       <c r="B103" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C103" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
@@ -1905,43 +1914,43 @@
         <v>85</v>
       </c>
       <c r="B104" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C104" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B105" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="C105" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B106" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="C106" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B107" t="s">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="C107" t="s">
-        <v>109</v>
+        <v>41</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -1949,10 +1958,10 @@
         <v>84</v>
       </c>
       <c r="B108" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C108" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
@@ -1960,10 +1969,10 @@
         <v>84</v>
       </c>
       <c r="B109" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C109" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -1971,10 +1980,10 @@
         <v>84</v>
       </c>
       <c r="B110" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C110" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
@@ -1982,10 +1991,10 @@
         <v>84</v>
       </c>
       <c r="B111" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C111" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -1993,10 +2002,10 @@
         <v>84</v>
       </c>
       <c r="B112" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C112" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
@@ -2004,9 +2013,42 @@
         <v>84</v>
       </c>
       <c r="B113" t="s">
+        <v>112</v>
+      </c>
+      <c r="C113" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>84</v>
+      </c>
+      <c r="B114" t="s">
+        <v>114</v>
+      </c>
+      <c r="C114" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>84</v>
+      </c>
+      <c r="B115" t="s">
+        <v>116</v>
+      </c>
+      <c r="C115" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>84</v>
+      </c>
+      <c r="B116" t="s">
         <v>118</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C116" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>